<commit_message>
Finished figures for simple LK fits I hope
</commit_message>
<xml_diff>
--- a/Chapter3-dHvABaFe2P2/Figures/Mass/MicroFits/Conversion.xlsx
+++ b/Chapter3-dHvABaFe2P2/Figures/Mass/MicroFits/Conversion.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="14">
   <si>
     <t>kCos(theta)</t>
   </si>
@@ -51,7 +51,13 @@
     <t>b3</t>
   </si>
   <si>
-    <t>d1</t>
+    <t>g2</t>
+  </si>
+  <si>
+    <t>a3</t>
+  </si>
+  <si>
+    <t>a3/d</t>
   </si>
 </sst>
 </file>
@@ -87,9 +93,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -384,13 +393,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="12.42578125" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" customWidth="1"/>
+    <col min="4" max="4" width="5.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
@@ -414,10 +428,10 @@
         <v>1210</v>
       </c>
       <c r="C2" s="1">
-        <f>COS(RADIANS(A2))*B2</f>
+        <f t="shared" ref="C2:C21" si="0">COS(RADIANS(A2))*B2</f>
         <v>1183.558596887905</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -429,10 +443,10 @@
         <v>1270</v>
       </c>
       <c r="C3" s="1">
-        <f>COS(RADIANS(A3))*B3</f>
+        <f t="shared" si="0"/>
         <v>1242.2474529319331</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="2" t="s">
         <v>5</v>
       </c>
     </row>
@@ -444,10 +458,10 @@
         <v>1372</v>
       </c>
       <c r="C4" s="1">
-        <f>COS(RADIANS(A4))*B4</f>
+        <f t="shared" si="0"/>
         <v>1342.0185082067815</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="2" t="s">
         <v>6</v>
       </c>
     </row>
@@ -459,10 +473,10 @@
         <v>2180</v>
       </c>
       <c r="C5" s="1">
-        <f>COS(RADIANS(A5))*B5</f>
+        <f t="shared" si="0"/>
         <v>2132.3617695996963</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="2" t="s">
         <v>7</v>
       </c>
     </row>
@@ -474,10 +488,10 @@
         <v>2350</v>
       </c>
       <c r="C6" s="1">
-        <f>COS(RADIANS(A6))*B6</f>
+        <f t="shared" si="0"/>
         <v>2298.6468617244432</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -489,10 +503,10 @@
         <v>912</v>
       </c>
       <c r="C7" s="1">
-        <f>COS(RADIANS(A7))*B7</f>
+        <f t="shared" si="0"/>
         <v>805.2482046873414</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="2" t="s">
         <v>9</v>
       </c>
     </row>
@@ -504,10 +518,10 @@
         <v>1269</v>
       </c>
       <c r="C8" s="1">
-        <f>COS(RADIANS(A8))*B8</f>
+        <f t="shared" si="0"/>
         <v>1120.4604953379783</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -519,11 +533,11 @@
         <v>1365</v>
       </c>
       <c r="C9" s="1">
-        <f>COS(RADIANS(A9))*B9</f>
+        <f t="shared" si="0"/>
         <v>1205.2234642524354</v>
       </c>
-      <c r="D9" t="s">
-        <v>5</v>
+      <c r="D9" s="2" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -534,10 +548,10 @@
         <v>1530</v>
       </c>
       <c r="C10" s="1">
-        <f>COS(RADIANS(A10))*B10</f>
+        <f t="shared" si="0"/>
         <v>1350.9098170741584</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="2" t="s">
         <v>6</v>
       </c>
     </row>
@@ -549,10 +563,10 @@
         <v>2475</v>
       </c>
       <c r="C11" s="1">
-        <f>COS(RADIANS(A11))*B11</f>
+        <f t="shared" si="0"/>
         <v>2185.2952923258445</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="2" t="s">
         <v>10</v>
       </c>
     </row>
@@ -564,10 +578,10 @@
         <v>2605</v>
       </c>
       <c r="C12" s="1">
-        <f>COS(RADIANS(A12))*B12</f>
+        <f t="shared" si="0"/>
         <v>2300.0784793975049</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -576,14 +590,14 @@
         <v>46</v>
       </c>
       <c r="B13">
-        <v>1532</v>
+        <v>1320</v>
       </c>
       <c r="C13" s="1">
-        <f>COS(RADIANS(A13))*B13</f>
-        <v>1064.2166235431837</v>
-      </c>
-      <c r="D13" t="s">
-        <v>4</v>
+        <f t="shared" si="0"/>
+        <v>916.94904900587642</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -591,14 +605,14 @@
         <v>46</v>
       </c>
       <c r="B14">
-        <v>1626</v>
+        <v>1532</v>
       </c>
       <c r="C14" s="1">
-        <f>COS(RADIANS(A14))*B14</f>
-        <v>1129.5145103663294</v>
-      </c>
-      <c r="D14" t="s">
-        <v>5</v>
+        <f t="shared" si="0"/>
+        <v>1064.2166235431837</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -606,14 +620,14 @@
         <v>46</v>
       </c>
       <c r="B15">
-        <v>2017</v>
+        <v>1626</v>
       </c>
       <c r="C15" s="1">
-        <f>COS(RADIANS(A15))*B15</f>
-        <v>1401.1259332157974</v>
-      </c>
-      <c r="D15" t="s">
-        <v>6</v>
+        <f t="shared" si="0"/>
+        <v>1129.5145103663294</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -621,14 +635,14 @@
         <v>46</v>
       </c>
       <c r="B16">
-        <v>2970</v>
+        <v>1930</v>
       </c>
       <c r="C16" s="1">
-        <f>COS(RADIANS(A16))*B16</f>
-        <v>2063.1353602632216</v>
-      </c>
-      <c r="D16" t="s">
-        <v>10</v>
+        <f t="shared" si="0"/>
+        <v>1340.6906549858647</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -636,14 +650,14 @@
         <v>46</v>
       </c>
       <c r="B17">
-        <v>3347</v>
+        <v>2017</v>
       </c>
       <c r="C17" s="1">
-        <f>COS(RADIANS(A17))*B17</f>
-        <v>2325.021565926264</v>
-      </c>
-      <c r="D17" t="s">
-        <v>8</v>
+        <f t="shared" si="0"/>
+        <v>1401.1259332157974</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -651,14 +665,14 @@
         <v>46</v>
       </c>
       <c r="B18">
-        <v>3381</v>
+        <v>2970</v>
       </c>
       <c r="C18" s="1">
-        <f>COS(RADIANS(A18))*B18</f>
-        <v>2348.6399505218697</v>
-      </c>
-      <c r="D18" t="s">
-        <v>8</v>
+        <f t="shared" si="0"/>
+        <v>2063.1353602632216</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -666,13 +680,43 @@
         <v>46</v>
       </c>
       <c r="B19">
+        <v>3347</v>
+      </c>
+      <c r="C19" s="1">
+        <f t="shared" si="0"/>
+        <v>2325.021565926264</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20">
+        <v>46</v>
+      </c>
+      <c r="B20">
+        <v>3381</v>
+      </c>
+      <c r="C20" s="1">
+        <f t="shared" si="0"/>
+        <v>2348.6399505218697</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21">
+        <v>46</v>
+      </c>
+      <c r="B21">
         <v>4497</v>
       </c>
-      <c r="C19" s="1">
-        <f>COS(RADIANS(A19))*B19</f>
+      <c r="C21" s="1">
+        <f t="shared" si="0"/>
         <v>3123.8786919541108</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D21" s="2" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>